<commit_message>
added petrol consumption calculations
</commit_message>
<xml_diff>
--- a/empty.xlsx
+++ b/empty.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\_1\python\cestaky\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8F7C65-3D48-4D06-850B-13916E04E1B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1162A6B8-2126-43F8-9003-5B150EEBA3AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -698,7 +698,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -847,6 +847,14 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -859,6 +867,14 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -895,6 +911,10 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
@@ -923,6 +943,14 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -947,6 +975,10 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -983,6 +1015,10 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1011,20 +1047,8 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1417,8 +1441,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ131"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15:H16"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H129" sqref="H129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1435,40 +1459,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="70" t="s">
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
       <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="85" t="s">
+      <c r="C2" s="45"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="85" t="s">
+      <c r="F2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="85" t="s">
+      <c r="G2" s="42" t="s">
         <v>12</v>
       </c>
       <c r="H2" s="5" t="s">
@@ -1491,15 +1515,15 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="84"/>
+      <c r="A3" s="48"/>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
       <c r="D3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
       <c r="H3" s="9" t="s">
         <v>10</v>
       </c>
@@ -1523,11 +1547,11 @@
       <c r="A4" s="11">
         <v>1</v>
       </c>
-      <c r="B4" s="72">
+      <c r="B4" s="80">
         <v>2</v>
       </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
       <c r="E4" s="12">
         <v>3</v>
       </c>
@@ -1557,1933 +1581,1933 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="73"/>
+      <c r="A5" s="81"/>
       <c r="B5" s="33"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="75"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="83"/>
       <c r="G5" s="15"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="75"/>
-      <c r="K5" s="75"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="76"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="85"/>
       <c r="N5" s="2"/>
     </row>
     <row r="6" spans="1:14" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="73"/>
+      <c r="A6" s="81"/>
       <c r="B6" s="22"/>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="75"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="83"/>
       <c r="G6" s="17"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
-      <c r="K6" s="75"/>
-      <c r="L6" s="71"/>
-      <c r="M6" s="76"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="83"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="85"/>
       <c r="N6" s="2"/>
     </row>
     <row r="7" spans="1:14" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="73"/>
+      <c r="A7" s="81"/>
       <c r="B7" s="22"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="66"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="73"/>
       <c r="G7" s="16"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="66"/>
-      <c r="J7" s="66"/>
-      <c r="K7" s="66"/>
-      <c r="L7" s="67"/>
-      <c r="M7" s="68"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="76"/>
       <c r="N7" s="2"/>
     </row>
     <row r="8" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="73"/>
+      <c r="A8" s="81"/>
       <c r="B8" s="18"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="66"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="73"/>
       <c r="G8" s="16"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="67"/>
-      <c r="M8" s="68"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="73"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="75"/>
+      <c r="M8" s="76"/>
       <c r="N8" s="2"/>
     </row>
     <row r="9" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="54"/>
+      <c r="A9" s="59"/>
       <c r="B9" s="34"/>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="53"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="57"/>
       <c r="G9" s="16"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="55"/>
-      <c r="M9" s="56"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="57"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="61"/>
       <c r="N9" s="2"/>
     </row>
     <row r="10" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="54"/>
+      <c r="A10" s="59"/>
       <c r="B10" s="22"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="53"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="57"/>
       <c r="G10" s="16"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="55"/>
-      <c r="M10" s="56"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="61"/>
       <c r="N10" s="2"/>
     </row>
     <row r="11" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="54"/>
+      <c r="A11" s="59"/>
       <c r="B11" s="22"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="66"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="73"/>
       <c r="G11" s="16"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="55"/>
-      <c r="M11" s="56"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="60"/>
+      <c r="M11" s="61"/>
       <c r="N11" s="2"/>
     </row>
     <row r="12" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="54"/>
+      <c r="A12" s="59"/>
       <c r="B12" s="18"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="66"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="73"/>
       <c r="G12" s="16"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="55"/>
-      <c r="M12" s="56"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="57"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="61"/>
       <c r="N12" s="2"/>
     </row>
     <row r="13" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="54"/>
+      <c r="A13" s="59"/>
       <c r="B13" s="34"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="53"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="57"/>
       <c r="G13" s="16"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="53"/>
-      <c r="L13" s="55"/>
-      <c r="M13" s="56"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="60"/>
+      <c r="M13" s="61"/>
       <c r="N13" s="2"/>
     </row>
     <row r="14" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="54"/>
+      <c r="A14" s="59"/>
       <c r="B14" s="22"/>
       <c r="C14" s="19"/>
       <c r="D14" s="16"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="53"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="57"/>
       <c r="G14" s="16"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="53"/>
-      <c r="L14" s="55"/>
-      <c r="M14" s="56"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="57"/>
+      <c r="K14" s="57"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="61"/>
       <c r="N14" s="2"/>
     </row>
     <row r="15" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="54"/>
+      <c r="A15" s="59"/>
       <c r="B15" s="22"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="66"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="73"/>
       <c r="G15" s="16"/>
-      <c r="H15" s="66"/>
-      <c r="I15" s="66"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="66"/>
-      <c r="L15" s="67"/>
-      <c r="M15" s="68"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="73"/>
+      <c r="J15" s="73"/>
+      <c r="K15" s="73"/>
+      <c r="L15" s="75"/>
+      <c r="M15" s="76"/>
       <c r="N15" s="2"/>
     </row>
     <row r="16" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="54"/>
+      <c r="A16" s="59"/>
       <c r="B16" s="18"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="66"/>
+      <c r="E16" s="72"/>
+      <c r="F16" s="73"/>
       <c r="G16" s="16"/>
-      <c r="H16" s="66"/>
-      <c r="I16" s="66"/>
-      <c r="J16" s="66"/>
-      <c r="K16" s="66"/>
-      <c r="L16" s="67"/>
-      <c r="M16" s="68"/>
+      <c r="H16" s="74"/>
+      <c r="I16" s="73"/>
+      <c r="J16" s="73"/>
+      <c r="K16" s="73"/>
+      <c r="L16" s="75"/>
+      <c r="M16" s="76"/>
       <c r="N16" s="2"/>
     </row>
     <row r="17" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="54"/>
+      <c r="A17" s="59"/>
       <c r="B17" s="34"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="53"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="57"/>
       <c r="G17" s="16"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="53"/>
-      <c r="L17" s="55"/>
-      <c r="M17" s="56"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="57"/>
+      <c r="K17" s="57"/>
+      <c r="L17" s="60"/>
+      <c r="M17" s="61"/>
       <c r="N17" s="2"/>
     </row>
     <row r="18" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="54"/>
+      <c r="A18" s="59"/>
       <c r="B18" s="22"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="53"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="57"/>
       <c r="G18" s="16"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="55"/>
-      <c r="M18" s="56"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="61"/>
       <c r="N18" s="2"/>
     </row>
     <row r="19" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="54"/>
+      <c r="A19" s="59"/>
       <c r="B19" s="22"/>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="66"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="73"/>
       <c r="G19" s="16"/>
-      <c r="H19" s="66"/>
-      <c r="I19" s="66"/>
-      <c r="J19" s="66"/>
-      <c r="K19" s="66"/>
-      <c r="L19" s="67"/>
-      <c r="M19" s="68"/>
+      <c r="H19" s="74"/>
+      <c r="I19" s="73"/>
+      <c r="J19" s="73"/>
+      <c r="K19" s="73"/>
+      <c r="L19" s="75"/>
+      <c r="M19" s="76"/>
       <c r="N19" s="2"/>
     </row>
     <row r="20" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="54"/>
+      <c r="A20" s="59"/>
       <c r="B20" s="18"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="66"/>
+      <c r="E20" s="72"/>
+      <c r="F20" s="73"/>
       <c r="G20" s="16"/>
-      <c r="H20" s="66"/>
-      <c r="I20" s="66"/>
-      <c r="J20" s="66"/>
-      <c r="K20" s="66"/>
-      <c r="L20" s="67"/>
-      <c r="M20" s="68"/>
+      <c r="H20" s="74"/>
+      <c r="I20" s="73"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="73"/>
+      <c r="L20" s="75"/>
+      <c r="M20" s="76"/>
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="54"/>
+      <c r="A21" s="59"/>
       <c r="B21" s="34"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="53"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="57"/>
       <c r="G21" s="16"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="53"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="55"/>
-      <c r="M21" s="56"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="60"/>
+      <c r="M21" s="61"/>
       <c r="N21" s="2"/>
     </row>
     <row r="22" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="54"/>
+      <c r="A22" s="59"/>
       <c r="B22" s="22"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="53"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="57"/>
       <c r="G22" s="16"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="53"/>
-      <c r="L22" s="55"/>
-      <c r="M22" s="56"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="57"/>
+      <c r="K22" s="57"/>
+      <c r="L22" s="60"/>
+      <c r="M22" s="61"/>
       <c r="N22" s="2"/>
     </row>
     <row r="23" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="54"/>
+      <c r="A23" s="59"/>
       <c r="B23" s="22"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="66"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="73"/>
       <c r="G23" s="16"/>
-      <c r="H23" s="66"/>
-      <c r="I23" s="66"/>
-      <c r="J23" s="66"/>
-      <c r="K23" s="66"/>
-      <c r="L23" s="67"/>
-      <c r="M23" s="68"/>
+      <c r="H23" s="74"/>
+      <c r="I23" s="73"/>
+      <c r="J23" s="73"/>
+      <c r="K23" s="73"/>
+      <c r="L23" s="75"/>
+      <c r="M23" s="76"/>
       <c r="N23" s="2"/>
     </row>
     <row r="24" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="54"/>
+      <c r="A24" s="59"/>
       <c r="B24" s="18"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="66"/>
+      <c r="E24" s="72"/>
+      <c r="F24" s="73"/>
       <c r="G24" s="19"/>
-      <c r="H24" s="66"/>
-      <c r="I24" s="66"/>
-      <c r="J24" s="66"/>
-      <c r="K24" s="66"/>
-      <c r="L24" s="67"/>
-      <c r="M24" s="68"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="73"/>
+      <c r="J24" s="73"/>
+      <c r="K24" s="73"/>
+      <c r="L24" s="75"/>
+      <c r="M24" s="76"/>
       <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="54"/>
+      <c r="A25" s="59"/>
       <c r="B25" s="34"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="53"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="57"/>
       <c r="G25" s="16"/>
-      <c r="H25" s="53"/>
-      <c r="I25" s="53"/>
-      <c r="J25" s="53"/>
-      <c r="K25" s="53"/>
-      <c r="L25" s="55"/>
-      <c r="M25" s="56"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="57"/>
+      <c r="J25" s="57"/>
+      <c r="K25" s="57"/>
+      <c r="L25" s="60"/>
+      <c r="M25" s="61"/>
       <c r="N25" s="2"/>
     </row>
     <row r="26" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="54"/>
+      <c r="A26" s="59"/>
       <c r="B26" s="22"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="53"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="57"/>
       <c r="G26" s="19"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="53"/>
-      <c r="K26" s="53"/>
-      <c r="L26" s="55"/>
-      <c r="M26" s="56"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="57"/>
+      <c r="K26" s="57"/>
+      <c r="L26" s="60"/>
+      <c r="M26" s="61"/>
       <c r="N26" s="2"/>
     </row>
     <row r="27" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="54"/>
+      <c r="A27" s="59"/>
       <c r="B27" s="22"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="66"/>
+      <c r="E27" s="72"/>
+      <c r="F27" s="73"/>
       <c r="G27" s="16"/>
-      <c r="H27" s="66"/>
-      <c r="I27" s="66"/>
-      <c r="J27" s="66"/>
-      <c r="K27" s="66"/>
-      <c r="L27" s="67"/>
-      <c r="M27" s="68"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="73"/>
+      <c r="J27" s="73"/>
+      <c r="K27" s="73"/>
+      <c r="L27" s="75"/>
+      <c r="M27" s="76"/>
       <c r="N27" s="2"/>
     </row>
     <row r="28" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="54"/>
+      <c r="A28" s="59"/>
       <c r="B28" s="18"/>
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
-      <c r="E28" s="65"/>
-      <c r="F28" s="66"/>
+      <c r="E28" s="72"/>
+      <c r="F28" s="73"/>
       <c r="G28" s="16"/>
-      <c r="H28" s="66"/>
-      <c r="I28" s="66"/>
-      <c r="J28" s="66"/>
-      <c r="K28" s="66"/>
-      <c r="L28" s="67"/>
-      <c r="M28" s="68"/>
+      <c r="H28" s="74"/>
+      <c r="I28" s="73"/>
+      <c r="J28" s="73"/>
+      <c r="K28" s="73"/>
+      <c r="L28" s="75"/>
+      <c r="M28" s="76"/>
       <c r="N28" s="2"/>
     </row>
     <row r="29" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="54"/>
+      <c r="A29" s="59"/>
       <c r="B29" s="34"/>
       <c r="C29" s="16"/>
       <c r="D29" s="16"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="53"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="57"/>
       <c r="G29" s="16"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="53"/>
-      <c r="J29" s="53"/>
-      <c r="K29" s="53"/>
-      <c r="L29" s="55"/>
-      <c r="M29" s="56"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="57"/>
+      <c r="J29" s="57"/>
+      <c r="K29" s="57"/>
+      <c r="L29" s="60"/>
+      <c r="M29" s="61"/>
       <c r="N29" s="2"/>
     </row>
     <row r="30" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="54"/>
+      <c r="A30" s="59"/>
       <c r="B30" s="22"/>
       <c r="C30" s="16"/>
       <c r="D30" s="16"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="53"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="57"/>
       <c r="G30" s="16"/>
-      <c r="H30" s="53"/>
-      <c r="I30" s="53"/>
-      <c r="J30" s="53"/>
-      <c r="K30" s="53"/>
-      <c r="L30" s="55"/>
-      <c r="M30" s="56"/>
+      <c r="H30" s="58"/>
+      <c r="I30" s="57"/>
+      <c r="J30" s="57"/>
+      <c r="K30" s="57"/>
+      <c r="L30" s="60"/>
+      <c r="M30" s="61"/>
       <c r="N30" s="2"/>
     </row>
     <row r="31" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="54"/>
+      <c r="A31" s="59"/>
       <c r="B31" s="22"/>
       <c r="C31" s="16"/>
       <c r="D31" s="16"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="66"/>
+      <c r="E31" s="72"/>
+      <c r="F31" s="73"/>
       <c r="G31" s="16"/>
-      <c r="H31" s="66"/>
-      <c r="I31" s="66"/>
-      <c r="J31" s="66"/>
-      <c r="K31" s="66"/>
-      <c r="L31" s="67"/>
-      <c r="M31" s="68"/>
+      <c r="H31" s="74"/>
+      <c r="I31" s="73"/>
+      <c r="J31" s="73"/>
+      <c r="K31" s="73"/>
+      <c r="L31" s="75"/>
+      <c r="M31" s="76"/>
       <c r="N31" s="2"/>
     </row>
     <row r="32" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="54"/>
+      <c r="A32" s="59"/>
       <c r="B32" s="18"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="66"/>
+      <c r="E32" s="72"/>
+      <c r="F32" s="73"/>
       <c r="G32" s="16"/>
-      <c r="H32" s="66"/>
-      <c r="I32" s="66"/>
-      <c r="J32" s="66"/>
-      <c r="K32" s="66"/>
-      <c r="L32" s="67"/>
-      <c r="M32" s="68"/>
+      <c r="H32" s="74"/>
+      <c r="I32" s="73"/>
+      <c r="J32" s="73"/>
+      <c r="K32" s="73"/>
+      <c r="L32" s="75"/>
+      <c r="M32" s="76"/>
       <c r="N32" s="2"/>
     </row>
     <row r="33" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="54"/>
+      <c r="A33" s="59"/>
       <c r="B33" s="34"/>
       <c r="C33" s="16"/>
       <c r="D33" s="16"/>
-      <c r="E33" s="52"/>
-      <c r="F33" s="53"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="57"/>
       <c r="G33" s="16"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="53"/>
-      <c r="J33" s="53"/>
-      <c r="K33" s="53"/>
-      <c r="L33" s="55"/>
-      <c r="M33" s="56"/>
+      <c r="H33" s="58"/>
+      <c r="I33" s="57"/>
+      <c r="J33" s="57"/>
+      <c r="K33" s="57"/>
+      <c r="L33" s="60"/>
+      <c r="M33" s="61"/>
       <c r="N33" s="2"/>
     </row>
     <row r="34" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="54"/>
+      <c r="A34" s="59"/>
       <c r="B34" s="22"/>
       <c r="C34" s="16"/>
       <c r="D34" s="16"/>
-      <c r="E34" s="52"/>
-      <c r="F34" s="53"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="57"/>
       <c r="G34" s="16"/>
-      <c r="H34" s="53"/>
-      <c r="I34" s="53"/>
-      <c r="J34" s="53"/>
-      <c r="K34" s="53"/>
-      <c r="L34" s="55"/>
-      <c r="M34" s="56"/>
+      <c r="H34" s="58"/>
+      <c r="I34" s="57"/>
+      <c r="J34" s="57"/>
+      <c r="K34" s="57"/>
+      <c r="L34" s="60"/>
+      <c r="M34" s="61"/>
       <c r="N34" s="2"/>
     </row>
     <row r="35" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="54"/>
+      <c r="A35" s="59"/>
       <c r="B35" s="22"/>
       <c r="C35" s="16"/>
       <c r="D35" s="16"/>
-      <c r="E35" s="65"/>
-      <c r="F35" s="66"/>
+      <c r="E35" s="72"/>
+      <c r="F35" s="73"/>
       <c r="G35" s="16"/>
-      <c r="H35" s="66"/>
-      <c r="I35" s="66"/>
-      <c r="J35" s="66"/>
-      <c r="K35" s="66"/>
-      <c r="L35" s="67"/>
-      <c r="M35" s="68"/>
+      <c r="H35" s="74"/>
+      <c r="I35" s="73"/>
+      <c r="J35" s="73"/>
+      <c r="K35" s="73"/>
+      <c r="L35" s="75"/>
+      <c r="M35" s="76"/>
       <c r="N35" s="2"/>
     </row>
     <row r="36" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="54"/>
+      <c r="A36" s="59"/>
       <c r="B36" s="18"/>
       <c r="C36" s="16"/>
       <c r="D36" s="16"/>
-      <c r="E36" s="65"/>
-      <c r="F36" s="66"/>
+      <c r="E36" s="72"/>
+      <c r="F36" s="73"/>
       <c r="G36" s="16"/>
-      <c r="H36" s="66"/>
-      <c r="I36" s="66"/>
-      <c r="J36" s="66"/>
-      <c r="K36" s="66"/>
-      <c r="L36" s="67"/>
-      <c r="M36" s="68"/>
+      <c r="H36" s="74"/>
+      <c r="I36" s="73"/>
+      <c r="J36" s="73"/>
+      <c r="K36" s="73"/>
+      <c r="L36" s="75"/>
+      <c r="M36" s="76"/>
       <c r="N36" s="2"/>
     </row>
     <row r="37" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="54"/>
+      <c r="A37" s="59"/>
       <c r="B37" s="34"/>
       <c r="C37" s="16"/>
       <c r="D37" s="16"/>
-      <c r="E37" s="52"/>
-      <c r="F37" s="53"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="57"/>
       <c r="G37" s="16"/>
-      <c r="H37" s="53"/>
-      <c r="I37" s="53"/>
-      <c r="J37" s="53"/>
-      <c r="K37" s="53"/>
-      <c r="L37" s="55"/>
-      <c r="M37" s="56"/>
+      <c r="H37" s="58"/>
+      <c r="I37" s="57"/>
+      <c r="J37" s="57"/>
+      <c r="K37" s="57"/>
+      <c r="L37" s="60"/>
+      <c r="M37" s="61"/>
       <c r="N37" s="2"/>
     </row>
     <row r="38" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="54"/>
+      <c r="A38" s="59"/>
       <c r="B38" s="22"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
-      <c r="E38" s="52"/>
-      <c r="F38" s="53"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="57"/>
       <c r="G38" s="16"/>
-      <c r="H38" s="53"/>
-      <c r="I38" s="53"/>
-      <c r="J38" s="53"/>
-      <c r="K38" s="53"/>
-      <c r="L38" s="55"/>
-      <c r="M38" s="56"/>
+      <c r="H38" s="58"/>
+      <c r="I38" s="57"/>
+      <c r="J38" s="57"/>
+      <c r="K38" s="57"/>
+      <c r="L38" s="60"/>
+      <c r="M38" s="61"/>
       <c r="N38" s="2"/>
     </row>
     <row r="39" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="54"/>
+      <c r="A39" s="59"/>
       <c r="B39" s="22"/>
       <c r="C39" s="16"/>
       <c r="D39" s="16"/>
-      <c r="E39" s="65"/>
-      <c r="F39" s="66"/>
+      <c r="E39" s="72"/>
+      <c r="F39" s="73"/>
       <c r="G39" s="16"/>
-      <c r="H39" s="66"/>
-      <c r="I39" s="66"/>
-      <c r="J39" s="66"/>
-      <c r="K39" s="66"/>
-      <c r="L39" s="67"/>
-      <c r="M39" s="68"/>
+      <c r="H39" s="74"/>
+      <c r="I39" s="73"/>
+      <c r="J39" s="73"/>
+      <c r="K39" s="73"/>
+      <c r="L39" s="75"/>
+      <c r="M39" s="76"/>
       <c r="N39" s="2"/>
     </row>
     <row r="40" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="54"/>
+      <c r="A40" s="59"/>
       <c r="B40" s="18"/>
       <c r="C40" s="16"/>
       <c r="D40" s="16"/>
-      <c r="E40" s="65"/>
-      <c r="F40" s="66"/>
+      <c r="E40" s="72"/>
+      <c r="F40" s="73"/>
       <c r="G40" s="16"/>
-      <c r="H40" s="66"/>
-      <c r="I40" s="66"/>
-      <c r="J40" s="66"/>
-      <c r="K40" s="66"/>
-      <c r="L40" s="67"/>
-      <c r="M40" s="68"/>
+      <c r="H40" s="74"/>
+      <c r="I40" s="73"/>
+      <c r="J40" s="73"/>
+      <c r="K40" s="73"/>
+      <c r="L40" s="75"/>
+      <c r="M40" s="76"/>
       <c r="N40" s="2"/>
     </row>
     <row r="41" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="54"/>
+      <c r="A41" s="59"/>
       <c r="B41" s="34"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
-      <c r="E41" s="52"/>
-      <c r="F41" s="53"/>
+      <c r="E41" s="56"/>
+      <c r="F41" s="57"/>
       <c r="G41" s="16"/>
-      <c r="H41" s="53"/>
-      <c r="I41" s="53"/>
-      <c r="J41" s="53"/>
-      <c r="K41" s="53"/>
-      <c r="L41" s="55"/>
-      <c r="M41" s="56"/>
+      <c r="H41" s="58"/>
+      <c r="I41" s="57"/>
+      <c r="J41" s="57"/>
+      <c r="K41" s="57"/>
+      <c r="L41" s="60"/>
+      <c r="M41" s="61"/>
       <c r="N41" s="2"/>
     </row>
     <row r="42" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="54"/>
+      <c r="A42" s="59"/>
       <c r="B42" s="22"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>
-      <c r="E42" s="52"/>
-      <c r="F42" s="53"/>
+      <c r="E42" s="56"/>
+      <c r="F42" s="57"/>
       <c r="G42" s="16"/>
-      <c r="H42" s="53"/>
-      <c r="I42" s="53"/>
-      <c r="J42" s="53"/>
-      <c r="K42" s="53"/>
-      <c r="L42" s="55"/>
-      <c r="M42" s="56"/>
+      <c r="H42" s="58"/>
+      <c r="I42" s="57"/>
+      <c r="J42" s="57"/>
+      <c r="K42" s="57"/>
+      <c r="L42" s="60"/>
+      <c r="M42" s="61"/>
       <c r="N42" s="2"/>
     </row>
     <row r="43" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="54"/>
+      <c r="A43" s="59"/>
       <c r="B43" s="22"/>
       <c r="C43" s="16"/>
       <c r="D43" s="16"/>
-      <c r="E43" s="65"/>
-      <c r="F43" s="66"/>
+      <c r="E43" s="72"/>
+      <c r="F43" s="73"/>
       <c r="G43" s="16"/>
-      <c r="H43" s="66"/>
-      <c r="I43" s="66"/>
-      <c r="J43" s="66"/>
-      <c r="K43" s="66"/>
-      <c r="L43" s="67"/>
-      <c r="M43" s="68"/>
+      <c r="H43" s="74"/>
+      <c r="I43" s="73"/>
+      <c r="J43" s="73"/>
+      <c r="K43" s="73"/>
+      <c r="L43" s="75"/>
+      <c r="M43" s="76"/>
       <c r="N43" s="2"/>
     </row>
     <row r="44" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="54"/>
+      <c r="A44" s="59"/>
       <c r="B44" s="18"/>
       <c r="C44" s="16"/>
       <c r="D44" s="16"/>
-      <c r="E44" s="65"/>
-      <c r="F44" s="66"/>
+      <c r="E44" s="72"/>
+      <c r="F44" s="73"/>
       <c r="G44" s="16"/>
-      <c r="H44" s="66"/>
-      <c r="I44" s="66"/>
-      <c r="J44" s="66"/>
-      <c r="K44" s="66"/>
-      <c r="L44" s="67"/>
-      <c r="M44" s="68"/>
+      <c r="H44" s="74"/>
+      <c r="I44" s="73"/>
+      <c r="J44" s="73"/>
+      <c r="K44" s="73"/>
+      <c r="L44" s="75"/>
+      <c r="M44" s="76"/>
       <c r="N44" s="2"/>
     </row>
     <row r="45" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="54"/>
+      <c r="A45" s="59"/>
       <c r="B45" s="34"/>
       <c r="C45" s="16"/>
       <c r="D45" s="16"/>
-      <c r="E45" s="52"/>
-      <c r="F45" s="53"/>
+      <c r="E45" s="56"/>
+      <c r="F45" s="57"/>
       <c r="G45" s="16"/>
-      <c r="H45" s="53"/>
-      <c r="I45" s="53"/>
-      <c r="J45" s="53"/>
-      <c r="K45" s="53"/>
-      <c r="L45" s="55"/>
-      <c r="M45" s="56"/>
+      <c r="H45" s="58"/>
+      <c r="I45" s="57"/>
+      <c r="J45" s="57"/>
+      <c r="K45" s="57"/>
+      <c r="L45" s="60"/>
+      <c r="M45" s="61"/>
       <c r="N45" s="2"/>
     </row>
     <row r="46" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="54"/>
+      <c r="A46" s="59"/>
       <c r="B46" s="22"/>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
-      <c r="E46" s="52"/>
-      <c r="F46" s="53"/>
+      <c r="E46" s="56"/>
+      <c r="F46" s="57"/>
       <c r="G46" s="16"/>
-      <c r="H46" s="53"/>
-      <c r="I46" s="53"/>
-      <c r="J46" s="53"/>
-      <c r="K46" s="53"/>
-      <c r="L46" s="55"/>
-      <c r="M46" s="56"/>
+      <c r="H46" s="58"/>
+      <c r="I46" s="57"/>
+      <c r="J46" s="57"/>
+      <c r="K46" s="57"/>
+      <c r="L46" s="60"/>
+      <c r="M46" s="61"/>
       <c r="N46" s="2"/>
     </row>
     <row r="47" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="54"/>
+      <c r="A47" s="59"/>
       <c r="B47" s="22"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
-      <c r="E47" s="65"/>
-      <c r="F47" s="53"/>
+      <c r="E47" s="72"/>
+      <c r="F47" s="57"/>
       <c r="G47" s="16"/>
-      <c r="H47" s="66"/>
-      <c r="I47" s="66"/>
-      <c r="J47" s="66"/>
-      <c r="K47" s="66"/>
-      <c r="L47" s="67"/>
-      <c r="M47" s="68"/>
+      <c r="H47" s="74"/>
+      <c r="I47" s="73"/>
+      <c r="J47" s="73"/>
+      <c r="K47" s="73"/>
+      <c r="L47" s="75"/>
+      <c r="M47" s="76"/>
       <c r="N47" s="2"/>
     </row>
     <row r="48" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="54"/>
+      <c r="A48" s="59"/>
       <c r="B48" s="18"/>
       <c r="C48" s="16"/>
       <c r="D48" s="16"/>
-      <c r="E48" s="65"/>
-      <c r="F48" s="53"/>
+      <c r="E48" s="72"/>
+      <c r="F48" s="57"/>
       <c r="G48" s="16"/>
-      <c r="H48" s="66"/>
-      <c r="I48" s="66"/>
-      <c r="J48" s="66"/>
-      <c r="K48" s="66"/>
-      <c r="L48" s="67"/>
-      <c r="M48" s="68"/>
+      <c r="H48" s="74"/>
+      <c r="I48" s="73"/>
+      <c r="J48" s="73"/>
+      <c r="K48" s="73"/>
+      <c r="L48" s="75"/>
+      <c r="M48" s="76"/>
       <c r="N48" s="2"/>
     </row>
     <row r="49" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="54"/>
+      <c r="A49" s="59"/>
       <c r="B49" s="34"/>
       <c r="C49" s="16"/>
       <c r="D49" s="16"/>
-      <c r="E49" s="52"/>
-      <c r="F49" s="53"/>
+      <c r="E49" s="56"/>
+      <c r="F49" s="57"/>
       <c r="G49" s="16"/>
-      <c r="H49" s="53"/>
-      <c r="I49" s="53"/>
-      <c r="J49" s="53"/>
-      <c r="K49" s="53"/>
-      <c r="L49" s="55"/>
-      <c r="M49" s="56"/>
+      <c r="H49" s="58"/>
+      <c r="I49" s="57"/>
+      <c r="J49" s="57"/>
+      <c r="K49" s="57"/>
+      <c r="L49" s="60"/>
+      <c r="M49" s="61"/>
       <c r="N49" s="2"/>
     </row>
     <row r="50" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="54"/>
+      <c r="A50" s="59"/>
       <c r="B50" s="22"/>
       <c r="C50" s="16"/>
       <c r="D50" s="16"/>
-      <c r="E50" s="52"/>
-      <c r="F50" s="53"/>
+      <c r="E50" s="56"/>
+      <c r="F50" s="57"/>
       <c r="G50" s="16"/>
-      <c r="H50" s="53"/>
-      <c r="I50" s="53"/>
-      <c r="J50" s="53"/>
-      <c r="K50" s="53"/>
-      <c r="L50" s="55"/>
-      <c r="M50" s="56"/>
+      <c r="H50" s="58"/>
+      <c r="I50" s="57"/>
+      <c r="J50" s="57"/>
+      <c r="K50" s="57"/>
+      <c r="L50" s="60"/>
+      <c r="M50" s="61"/>
       <c r="N50" s="2"/>
     </row>
     <row r="51" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="54"/>
+      <c r="A51" s="59"/>
       <c r="B51" s="22"/>
       <c r="C51" s="16"/>
       <c r="D51" s="16"/>
-      <c r="E51" s="65"/>
-      <c r="F51" s="66"/>
+      <c r="E51" s="72"/>
+      <c r="F51" s="73"/>
       <c r="G51" s="16"/>
-      <c r="H51" s="66"/>
-      <c r="I51" s="66"/>
-      <c r="J51" s="66"/>
-      <c r="K51" s="66"/>
-      <c r="L51" s="67"/>
-      <c r="M51" s="68"/>
+      <c r="H51" s="74"/>
+      <c r="I51" s="73"/>
+      <c r="J51" s="73"/>
+      <c r="K51" s="73"/>
+      <c r="L51" s="75"/>
+      <c r="M51" s="76"/>
       <c r="N51" s="2"/>
     </row>
     <row r="52" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="54"/>
+      <c r="A52" s="59"/>
       <c r="B52" s="18"/>
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
-      <c r="E52" s="65"/>
-      <c r="F52" s="66"/>
+      <c r="E52" s="72"/>
+      <c r="F52" s="73"/>
       <c r="G52" s="16"/>
-      <c r="H52" s="66"/>
-      <c r="I52" s="66"/>
-      <c r="J52" s="66"/>
-      <c r="K52" s="66"/>
-      <c r="L52" s="67"/>
-      <c r="M52" s="68"/>
+      <c r="H52" s="74"/>
+      <c r="I52" s="73"/>
+      <c r="J52" s="73"/>
+      <c r="K52" s="73"/>
+      <c r="L52" s="75"/>
+      <c r="M52" s="76"/>
       <c r="N52" s="2"/>
     </row>
     <row r="53" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="54"/>
+      <c r="A53" s="59"/>
       <c r="B53" s="34"/>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
-      <c r="E53" s="52"/>
-      <c r="F53" s="53"/>
+      <c r="E53" s="56"/>
+      <c r="F53" s="57"/>
       <c r="G53" s="16"/>
-      <c r="H53" s="53"/>
-      <c r="I53" s="53"/>
-      <c r="J53" s="53"/>
-      <c r="K53" s="53"/>
-      <c r="L53" s="55"/>
-      <c r="M53" s="56"/>
+      <c r="H53" s="58"/>
+      <c r="I53" s="57"/>
+      <c r="J53" s="57"/>
+      <c r="K53" s="57"/>
+      <c r="L53" s="60"/>
+      <c r="M53" s="61"/>
       <c r="N53" s="2"/>
     </row>
     <row r="54" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="54"/>
+      <c r="A54" s="59"/>
       <c r="B54" s="22"/>
       <c r="C54" s="16"/>
       <c r="D54" s="16"/>
-      <c r="E54" s="52"/>
-      <c r="F54" s="53"/>
+      <c r="E54" s="56"/>
+      <c r="F54" s="57"/>
       <c r="G54" s="16"/>
-      <c r="H54" s="53"/>
-      <c r="I54" s="53"/>
-      <c r="J54" s="53"/>
-      <c r="K54" s="53"/>
-      <c r="L54" s="55"/>
-      <c r="M54" s="56"/>
+      <c r="H54" s="58"/>
+      <c r="I54" s="57"/>
+      <c r="J54" s="57"/>
+      <c r="K54" s="57"/>
+      <c r="L54" s="60"/>
+      <c r="M54" s="61"/>
       <c r="N54" s="2"/>
     </row>
     <row r="55" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="54"/>
+      <c r="A55" s="59"/>
       <c r="B55" s="22"/>
       <c r="C55" s="16"/>
       <c r="D55" s="16"/>
-      <c r="E55" s="65"/>
-      <c r="F55" s="66"/>
+      <c r="E55" s="72"/>
+      <c r="F55" s="73"/>
       <c r="G55" s="16"/>
-      <c r="H55" s="66"/>
-      <c r="I55" s="66"/>
-      <c r="J55" s="66"/>
-      <c r="K55" s="66"/>
-      <c r="L55" s="67"/>
-      <c r="M55" s="68"/>
+      <c r="H55" s="74"/>
+      <c r="I55" s="73"/>
+      <c r="J55" s="73"/>
+      <c r="K55" s="73"/>
+      <c r="L55" s="75"/>
+      <c r="M55" s="76"/>
       <c r="N55" s="2"/>
     </row>
     <row r="56" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="54"/>
+      <c r="A56" s="59"/>
       <c r="B56" s="18"/>
       <c r="C56" s="16"/>
       <c r="D56" s="16"/>
-      <c r="E56" s="65"/>
-      <c r="F56" s="66"/>
+      <c r="E56" s="72"/>
+      <c r="F56" s="73"/>
       <c r="G56" s="19"/>
-      <c r="H56" s="66"/>
-      <c r="I56" s="66"/>
-      <c r="J56" s="66"/>
-      <c r="K56" s="66"/>
-      <c r="L56" s="67"/>
-      <c r="M56" s="68"/>
+      <c r="H56" s="74"/>
+      <c r="I56" s="73"/>
+      <c r="J56" s="73"/>
+      <c r="K56" s="73"/>
+      <c r="L56" s="75"/>
+      <c r="M56" s="76"/>
       <c r="N56" s="2"/>
     </row>
     <row r="57" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="54"/>
+      <c r="A57" s="59"/>
       <c r="B57" s="34"/>
       <c r="C57" s="16"/>
       <c r="D57" s="16"/>
-      <c r="E57" s="52"/>
-      <c r="F57" s="53"/>
+      <c r="E57" s="56"/>
+      <c r="F57" s="57"/>
       <c r="G57" s="16"/>
-      <c r="H57" s="53"/>
-      <c r="I57" s="53"/>
-      <c r="J57" s="53"/>
-      <c r="K57" s="53"/>
-      <c r="L57" s="55"/>
-      <c r="M57" s="56"/>
+      <c r="H57" s="58"/>
+      <c r="I57" s="57"/>
+      <c r="J57" s="57"/>
+      <c r="K57" s="57"/>
+      <c r="L57" s="60"/>
+      <c r="M57" s="61"/>
       <c r="N57" s="2"/>
     </row>
     <row r="58" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="54"/>
+      <c r="A58" s="59"/>
       <c r="B58" s="35"/>
       <c r="C58" s="16"/>
       <c r="D58" s="16"/>
-      <c r="E58" s="52"/>
-      <c r="F58" s="53"/>
+      <c r="E58" s="56"/>
+      <c r="F58" s="57"/>
       <c r="G58" s="16"/>
-      <c r="H58" s="53"/>
-      <c r="I58" s="53"/>
-      <c r="J58" s="53"/>
-      <c r="K58" s="53"/>
-      <c r="L58" s="55"/>
-      <c r="M58" s="56"/>
+      <c r="H58" s="58"/>
+      <c r="I58" s="57"/>
+      <c r="J58" s="57"/>
+      <c r="K58" s="57"/>
+      <c r="L58" s="60"/>
+      <c r="M58" s="61"/>
       <c r="N58" s="3"/>
     </row>
     <row r="59" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="54"/>
+      <c r="A59" s="59"/>
       <c r="B59" s="35"/>
       <c r="C59" s="16"/>
       <c r="D59" s="16"/>
-      <c r="E59" s="69"/>
-      <c r="F59" s="66"/>
+      <c r="E59" s="77"/>
+      <c r="F59" s="73"/>
       <c r="G59" s="19"/>
-      <c r="H59" s="66"/>
-      <c r="I59" s="66"/>
-      <c r="J59" s="66"/>
-      <c r="K59" s="66"/>
-      <c r="L59" s="67"/>
-      <c r="M59" s="68"/>
+      <c r="H59" s="74"/>
+      <c r="I59" s="73"/>
+      <c r="J59" s="73"/>
+      <c r="K59" s="73"/>
+      <c r="L59" s="75"/>
+      <c r="M59" s="76"/>
       <c r="N59" s="3"/>
     </row>
     <row r="60" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="54"/>
+      <c r="A60" s="59"/>
       <c r="B60" s="18"/>
       <c r="C60" s="16"/>
       <c r="D60" s="16"/>
-      <c r="E60" s="69"/>
-      <c r="F60" s="66"/>
+      <c r="E60" s="77"/>
+      <c r="F60" s="73"/>
       <c r="G60" s="19"/>
-      <c r="H60" s="66"/>
-      <c r="I60" s="66"/>
-      <c r="J60" s="66"/>
-      <c r="K60" s="66"/>
-      <c r="L60" s="67"/>
-      <c r="M60" s="68"/>
+      <c r="H60" s="74"/>
+      <c r="I60" s="73"/>
+      <c r="J60" s="73"/>
+      <c r="K60" s="73"/>
+      <c r="L60" s="75"/>
+      <c r="M60" s="76"/>
       <c r="N60" s="3"/>
     </row>
     <row r="61" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="54"/>
+      <c r="A61" s="59"/>
       <c r="B61" s="34"/>
       <c r="C61" s="16"/>
       <c r="D61" s="16"/>
-      <c r="E61" s="52"/>
-      <c r="F61" s="53"/>
+      <c r="E61" s="56"/>
+      <c r="F61" s="57"/>
       <c r="G61" s="16"/>
-      <c r="H61" s="53"/>
-      <c r="I61" s="53"/>
-      <c r="J61" s="53"/>
-      <c r="K61" s="53"/>
-      <c r="L61" s="55"/>
-      <c r="M61" s="56"/>
+      <c r="H61" s="58"/>
+      <c r="I61" s="57"/>
+      <c r="J61" s="57"/>
+      <c r="K61" s="57"/>
+      <c r="L61" s="60"/>
+      <c r="M61" s="61"/>
       <c r="N61" s="3"/>
     </row>
     <row r="62" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="54"/>
+      <c r="A62" s="59"/>
       <c r="B62" s="22"/>
       <c r="C62" s="16"/>
       <c r="D62" s="16"/>
-      <c r="E62" s="52"/>
-      <c r="F62" s="53"/>
+      <c r="E62" s="56"/>
+      <c r="F62" s="57"/>
       <c r="G62" s="16"/>
-      <c r="H62" s="53"/>
-      <c r="I62" s="53"/>
-      <c r="J62" s="53"/>
-      <c r="K62" s="53"/>
-      <c r="L62" s="55"/>
-      <c r="M62" s="56"/>
+      <c r="H62" s="58"/>
+      <c r="I62" s="57"/>
+      <c r="J62" s="57"/>
+      <c r="K62" s="57"/>
+      <c r="L62" s="60"/>
+      <c r="M62" s="61"/>
       <c r="N62" s="3"/>
     </row>
     <row r="63" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="54"/>
+      <c r="A63" s="59"/>
       <c r="B63" s="22"/>
       <c r="C63" s="16"/>
       <c r="D63" s="16"/>
-      <c r="E63" s="65"/>
-      <c r="F63" s="66"/>
+      <c r="E63" s="72"/>
+      <c r="F63" s="73"/>
       <c r="G63" s="16"/>
-      <c r="H63" s="66"/>
-      <c r="I63" s="66"/>
-      <c r="J63" s="66"/>
-      <c r="K63" s="66"/>
-      <c r="L63" s="67"/>
-      <c r="M63" s="68"/>
+      <c r="H63" s="74"/>
+      <c r="I63" s="73"/>
+      <c r="J63" s="73"/>
+      <c r="K63" s="73"/>
+      <c r="L63" s="75"/>
+      <c r="M63" s="76"/>
       <c r="N63" s="3"/>
     </row>
     <row r="64" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="54"/>
+      <c r="A64" s="59"/>
       <c r="B64" s="18"/>
       <c r="C64" s="16"/>
       <c r="D64" s="16"/>
-      <c r="E64" s="65"/>
-      <c r="F64" s="66"/>
+      <c r="E64" s="72"/>
+      <c r="F64" s="73"/>
       <c r="G64" s="19"/>
-      <c r="H64" s="66"/>
-      <c r="I64" s="66"/>
-      <c r="J64" s="66"/>
-      <c r="K64" s="66"/>
-      <c r="L64" s="67"/>
-      <c r="M64" s="68"/>
+      <c r="H64" s="74"/>
+      <c r="I64" s="73"/>
+      <c r="J64" s="73"/>
+      <c r="K64" s="73"/>
+      <c r="L64" s="75"/>
+      <c r="M64" s="76"/>
       <c r="N64" s="3"/>
     </row>
     <row r="65" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="54"/>
+      <c r="A65" s="59"/>
       <c r="B65" s="34"/>
       <c r="C65" s="16"/>
       <c r="D65" s="16"/>
-      <c r="E65" s="52"/>
-      <c r="F65" s="53"/>
+      <c r="E65" s="56"/>
+      <c r="F65" s="57"/>
       <c r="G65" s="16"/>
-      <c r="H65" s="53"/>
-      <c r="I65" s="53"/>
-      <c r="J65" s="53"/>
-      <c r="K65" s="53"/>
-      <c r="L65" s="55"/>
-      <c r="M65" s="56"/>
+      <c r="H65" s="58"/>
+      <c r="I65" s="57"/>
+      <c r="J65" s="57"/>
+      <c r="K65" s="57"/>
+      <c r="L65" s="60"/>
+      <c r="M65" s="61"/>
       <c r="N65" s="3"/>
     </row>
     <row r="66" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="54"/>
+      <c r="A66" s="59"/>
       <c r="B66" s="22"/>
       <c r="C66" s="16"/>
       <c r="D66" s="16"/>
-      <c r="E66" s="52"/>
-      <c r="F66" s="53"/>
+      <c r="E66" s="56"/>
+      <c r="F66" s="57"/>
       <c r="G66" s="16"/>
-      <c r="H66" s="53"/>
-      <c r="I66" s="53"/>
-      <c r="J66" s="53"/>
-      <c r="K66" s="53"/>
-      <c r="L66" s="55"/>
-      <c r="M66" s="56"/>
+      <c r="H66" s="58"/>
+      <c r="I66" s="57"/>
+      <c r="J66" s="57"/>
+      <c r="K66" s="57"/>
+      <c r="L66" s="60"/>
+      <c r="M66" s="61"/>
       <c r="N66" s="3"/>
     </row>
     <row r="67" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="54"/>
+      <c r="A67" s="59"/>
       <c r="B67" s="22"/>
       <c r="C67" s="16"/>
       <c r="D67" s="16"/>
-      <c r="E67" s="65"/>
-      <c r="F67" s="66"/>
+      <c r="E67" s="72"/>
+      <c r="F67" s="73"/>
       <c r="G67" s="16"/>
-      <c r="H67" s="66"/>
-      <c r="I67" s="66"/>
-      <c r="J67" s="66"/>
-      <c r="K67" s="66"/>
-      <c r="L67" s="67"/>
-      <c r="M67" s="68"/>
+      <c r="H67" s="74"/>
+      <c r="I67" s="73"/>
+      <c r="J67" s="73"/>
+      <c r="K67" s="73"/>
+      <c r="L67" s="75"/>
+      <c r="M67" s="76"/>
       <c r="N67" s="3"/>
     </row>
     <row r="68" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="54"/>
+      <c r="A68" s="59"/>
       <c r="B68" s="18"/>
       <c r="C68" s="16"/>
       <c r="D68" s="16"/>
-      <c r="E68" s="65"/>
-      <c r="F68" s="66"/>
+      <c r="E68" s="72"/>
+      <c r="F68" s="73"/>
       <c r="G68" s="16"/>
-      <c r="H68" s="66"/>
-      <c r="I68" s="66"/>
-      <c r="J68" s="66"/>
-      <c r="K68" s="66"/>
-      <c r="L68" s="67"/>
-      <c r="M68" s="68"/>
+      <c r="H68" s="74"/>
+      <c r="I68" s="73"/>
+      <c r="J68" s="73"/>
+      <c r="K68" s="73"/>
+      <c r="L68" s="75"/>
+      <c r="M68" s="76"/>
       <c r="N68" s="3"/>
     </row>
     <row r="69" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="54"/>
+      <c r="A69" s="59"/>
       <c r="B69" s="34"/>
       <c r="C69" s="16"/>
       <c r="D69" s="16"/>
-      <c r="E69" s="52"/>
-      <c r="F69" s="53"/>
+      <c r="E69" s="56"/>
+      <c r="F69" s="57"/>
       <c r="G69" s="16"/>
-      <c r="H69" s="53"/>
-      <c r="I69" s="53"/>
-      <c r="J69" s="53"/>
-      <c r="K69" s="53"/>
-      <c r="L69" s="55"/>
-      <c r="M69" s="56"/>
+      <c r="H69" s="58"/>
+      <c r="I69" s="57"/>
+      <c r="J69" s="57"/>
+      <c r="K69" s="57"/>
+      <c r="L69" s="60"/>
+      <c r="M69" s="61"/>
       <c r="N69" s="3"/>
     </row>
     <row r="70" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="54"/>
+      <c r="A70" s="59"/>
       <c r="B70" s="22"/>
       <c r="C70" s="16"/>
       <c r="D70" s="16"/>
-      <c r="E70" s="52"/>
-      <c r="F70" s="53"/>
+      <c r="E70" s="56"/>
+      <c r="F70" s="57"/>
       <c r="G70" s="16"/>
-      <c r="H70" s="53"/>
-      <c r="I70" s="53"/>
-      <c r="J70" s="53"/>
-      <c r="K70" s="53"/>
-      <c r="L70" s="55"/>
-      <c r="M70" s="56"/>
+      <c r="H70" s="58"/>
+      <c r="I70" s="57"/>
+      <c r="J70" s="57"/>
+      <c r="K70" s="57"/>
+      <c r="L70" s="60"/>
+      <c r="M70" s="61"/>
       <c r="N70" s="3"/>
     </row>
     <row r="71" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="54"/>
+      <c r="A71" s="59"/>
       <c r="B71" s="22"/>
       <c r="C71" s="16"/>
       <c r="D71" s="16"/>
-      <c r="E71" s="65"/>
-      <c r="F71" s="66"/>
+      <c r="E71" s="72"/>
+      <c r="F71" s="73"/>
       <c r="G71" s="16"/>
-      <c r="H71" s="66"/>
-      <c r="I71" s="66"/>
-      <c r="J71" s="66"/>
-      <c r="K71" s="66"/>
-      <c r="L71" s="67"/>
-      <c r="M71" s="68"/>
+      <c r="H71" s="74"/>
+      <c r="I71" s="73"/>
+      <c r="J71" s="73"/>
+      <c r="K71" s="73"/>
+      <c r="L71" s="75"/>
+      <c r="M71" s="76"/>
     </row>
     <row r="72" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="54"/>
+      <c r="A72" s="59"/>
       <c r="B72" s="18"/>
       <c r="C72" s="16"/>
       <c r="D72" s="16"/>
-      <c r="E72" s="65"/>
-      <c r="F72" s="66"/>
+      <c r="E72" s="72"/>
+      <c r="F72" s="73"/>
       <c r="G72" s="16"/>
-      <c r="H72" s="66"/>
-      <c r="I72" s="66"/>
-      <c r="J72" s="66"/>
-      <c r="K72" s="66"/>
-      <c r="L72" s="67"/>
-      <c r="M72" s="68"/>
+      <c r="H72" s="74"/>
+      <c r="I72" s="73"/>
+      <c r="J72" s="73"/>
+      <c r="K72" s="73"/>
+      <c r="L72" s="75"/>
+      <c r="M72" s="76"/>
     </row>
     <row r="73" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="54"/>
+      <c r="A73" s="59"/>
       <c r="B73" s="34"/>
       <c r="C73" s="16"/>
       <c r="D73" s="16"/>
-      <c r="E73" s="52"/>
-      <c r="F73" s="53"/>
+      <c r="E73" s="56"/>
+      <c r="F73" s="57"/>
       <c r="G73" s="16"/>
-      <c r="H73" s="53"/>
-      <c r="I73" s="53"/>
-      <c r="J73" s="53"/>
-      <c r="K73" s="53"/>
-      <c r="L73" s="55"/>
-      <c r="M73" s="56"/>
+      <c r="H73" s="58"/>
+      <c r="I73" s="57"/>
+      <c r="J73" s="57"/>
+      <c r="K73" s="57"/>
+      <c r="L73" s="60"/>
+      <c r="M73" s="61"/>
     </row>
     <row r="74" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="54"/>
+      <c r="A74" s="59"/>
       <c r="B74" s="22"/>
       <c r="C74" s="16"/>
       <c r="D74" s="16"/>
-      <c r="E74" s="52"/>
-      <c r="F74" s="53"/>
+      <c r="E74" s="56"/>
+      <c r="F74" s="57"/>
       <c r="G74" s="16"/>
-      <c r="H74" s="53"/>
-      <c r="I74" s="53"/>
-      <c r="J74" s="53"/>
-      <c r="K74" s="53"/>
-      <c r="L74" s="55"/>
-      <c r="M74" s="56"/>
+      <c r="H74" s="58"/>
+      <c r="I74" s="57"/>
+      <c r="J74" s="57"/>
+      <c r="K74" s="57"/>
+      <c r="L74" s="60"/>
+      <c r="M74" s="61"/>
     </row>
     <row r="75" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="54"/>
+      <c r="A75" s="59"/>
       <c r="B75" s="22"/>
       <c r="C75" s="16"/>
       <c r="D75" s="16"/>
-      <c r="E75" s="65"/>
-      <c r="F75" s="66"/>
+      <c r="E75" s="72"/>
+      <c r="F75" s="73"/>
       <c r="G75" s="16"/>
-      <c r="H75" s="66"/>
-      <c r="I75" s="66"/>
-      <c r="J75" s="66"/>
-      <c r="K75" s="66"/>
-      <c r="L75" s="67"/>
-      <c r="M75" s="68"/>
+      <c r="H75" s="74"/>
+      <c r="I75" s="73"/>
+      <c r="J75" s="73"/>
+      <c r="K75" s="73"/>
+      <c r="L75" s="75"/>
+      <c r="M75" s="76"/>
     </row>
     <row r="76" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="54"/>
+      <c r="A76" s="59"/>
       <c r="B76" s="18"/>
       <c r="C76" s="16"/>
       <c r="D76" s="16"/>
-      <c r="E76" s="65"/>
-      <c r="F76" s="66"/>
+      <c r="E76" s="72"/>
+      <c r="F76" s="73"/>
       <c r="G76" s="16"/>
-      <c r="H76" s="66"/>
-      <c r="I76" s="66"/>
-      <c r="J76" s="66"/>
-      <c r="K76" s="66"/>
-      <c r="L76" s="67"/>
-      <c r="M76" s="68"/>
+      <c r="H76" s="74"/>
+      <c r="I76" s="73"/>
+      <c r="J76" s="73"/>
+      <c r="K76" s="73"/>
+      <c r="L76" s="75"/>
+      <c r="M76" s="76"/>
     </row>
     <row r="77" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="54"/>
+      <c r="A77" s="59"/>
       <c r="B77" s="34"/>
       <c r="C77" s="16"/>
       <c r="D77" s="16"/>
-      <c r="E77" s="52"/>
-      <c r="F77" s="53"/>
+      <c r="E77" s="56"/>
+      <c r="F77" s="57"/>
       <c r="G77" s="16"/>
-      <c r="H77" s="53"/>
-      <c r="I77" s="53"/>
-      <c r="J77" s="53"/>
-      <c r="K77" s="53"/>
-      <c r="L77" s="55"/>
-      <c r="M77" s="56"/>
+      <c r="H77" s="58"/>
+      <c r="I77" s="57"/>
+      <c r="J77" s="57"/>
+      <c r="K77" s="57"/>
+      <c r="L77" s="60"/>
+      <c r="M77" s="61"/>
     </row>
     <row r="78" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="54"/>
+      <c r="A78" s="59"/>
       <c r="B78" s="22"/>
       <c r="C78" s="16"/>
       <c r="D78" s="16"/>
-      <c r="E78" s="52"/>
-      <c r="F78" s="53"/>
+      <c r="E78" s="56"/>
+      <c r="F78" s="57"/>
       <c r="G78" s="16"/>
-      <c r="H78" s="53"/>
-      <c r="I78" s="53"/>
-      <c r="J78" s="53"/>
-      <c r="K78" s="53"/>
-      <c r="L78" s="55"/>
-      <c r="M78" s="56"/>
+      <c r="H78" s="58"/>
+      <c r="I78" s="57"/>
+      <c r="J78" s="57"/>
+      <c r="K78" s="57"/>
+      <c r="L78" s="60"/>
+      <c r="M78" s="61"/>
     </row>
     <row r="79" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="54"/>
+      <c r="A79" s="59"/>
       <c r="B79" s="22"/>
       <c r="C79" s="16"/>
       <c r="D79" s="16"/>
-      <c r="E79" s="65"/>
-      <c r="F79" s="66"/>
+      <c r="E79" s="72"/>
+      <c r="F79" s="73"/>
       <c r="G79" s="16"/>
-      <c r="H79" s="66"/>
-      <c r="I79" s="66"/>
-      <c r="J79" s="66"/>
-      <c r="K79" s="66"/>
-      <c r="L79" s="67"/>
-      <c r="M79" s="68"/>
+      <c r="H79" s="74"/>
+      <c r="I79" s="73"/>
+      <c r="J79" s="73"/>
+      <c r="K79" s="73"/>
+      <c r="L79" s="75"/>
+      <c r="M79" s="76"/>
     </row>
     <row r="80" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="54"/>
+      <c r="A80" s="59"/>
       <c r="B80" s="18"/>
       <c r="C80" s="16"/>
       <c r="D80" s="16"/>
-      <c r="E80" s="65"/>
-      <c r="F80" s="66"/>
+      <c r="E80" s="72"/>
+      <c r="F80" s="73"/>
       <c r="G80" s="16"/>
-      <c r="H80" s="66"/>
-      <c r="I80" s="66"/>
-      <c r="J80" s="66"/>
-      <c r="K80" s="66"/>
-      <c r="L80" s="67"/>
-      <c r="M80" s="68"/>
+      <c r="H80" s="74"/>
+      <c r="I80" s="73"/>
+      <c r="J80" s="73"/>
+      <c r="K80" s="73"/>
+      <c r="L80" s="75"/>
+      <c r="M80" s="76"/>
     </row>
     <row r="81" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="54"/>
+      <c r="A81" s="59"/>
       <c r="B81" s="34"/>
       <c r="C81" s="16"/>
       <c r="D81" s="16"/>
-      <c r="E81" s="52"/>
-      <c r="F81" s="53"/>
+      <c r="E81" s="56"/>
+      <c r="F81" s="57"/>
       <c r="G81" s="16"/>
-      <c r="H81" s="53"/>
-      <c r="I81" s="53"/>
-      <c r="J81" s="53"/>
-      <c r="K81" s="53"/>
-      <c r="L81" s="55"/>
-      <c r="M81" s="56"/>
+      <c r="H81" s="58"/>
+      <c r="I81" s="57"/>
+      <c r="J81" s="57"/>
+      <c r="K81" s="57"/>
+      <c r="L81" s="60"/>
+      <c r="M81" s="61"/>
     </row>
     <row r="82" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="54"/>
+      <c r="A82" s="59"/>
       <c r="B82" s="22"/>
       <c r="C82" s="16"/>
       <c r="D82" s="16"/>
-      <c r="E82" s="52"/>
-      <c r="F82" s="53"/>
+      <c r="E82" s="56"/>
+      <c r="F82" s="57"/>
       <c r="G82" s="16"/>
-      <c r="H82" s="53"/>
-      <c r="I82" s="53"/>
-      <c r="J82" s="53"/>
-      <c r="K82" s="53"/>
-      <c r="L82" s="55"/>
-      <c r="M82" s="56"/>
+      <c r="H82" s="58"/>
+      <c r="I82" s="57"/>
+      <c r="J82" s="57"/>
+      <c r="K82" s="57"/>
+      <c r="L82" s="60"/>
+      <c r="M82" s="61"/>
     </row>
     <row r="83" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="54"/>
+      <c r="A83" s="59"/>
       <c r="B83" s="22"/>
       <c r="C83" s="16"/>
       <c r="D83" s="16"/>
-      <c r="E83" s="65"/>
-      <c r="F83" s="66"/>
+      <c r="E83" s="72"/>
+      <c r="F83" s="73"/>
       <c r="G83" s="16"/>
-      <c r="H83" s="66"/>
-      <c r="I83" s="66"/>
-      <c r="J83" s="66"/>
-      <c r="K83" s="66"/>
-      <c r="L83" s="67"/>
-      <c r="M83" s="68"/>
+      <c r="H83" s="74"/>
+      <c r="I83" s="73"/>
+      <c r="J83" s="73"/>
+      <c r="K83" s="73"/>
+      <c r="L83" s="75"/>
+      <c r="M83" s="76"/>
     </row>
     <row r="84" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="54"/>
+      <c r="A84" s="59"/>
       <c r="B84" s="18"/>
       <c r="C84" s="19"/>
       <c r="D84" s="16"/>
-      <c r="E84" s="65"/>
-      <c r="F84" s="66"/>
+      <c r="E84" s="72"/>
+      <c r="F84" s="73"/>
       <c r="G84" s="16"/>
-      <c r="H84" s="66"/>
-      <c r="I84" s="66"/>
-      <c r="J84" s="66"/>
-      <c r="K84" s="66"/>
-      <c r="L84" s="67"/>
-      <c r="M84" s="68"/>
+      <c r="H84" s="74"/>
+      <c r="I84" s="73"/>
+      <c r="J84" s="73"/>
+      <c r="K84" s="73"/>
+      <c r="L84" s="75"/>
+      <c r="M84" s="76"/>
     </row>
     <row r="85" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="54"/>
+      <c r="A85" s="59"/>
       <c r="B85" s="34"/>
       <c r="C85" s="16"/>
       <c r="D85" s="16"/>
-      <c r="E85" s="52"/>
-      <c r="F85" s="53"/>
+      <c r="E85" s="56"/>
+      <c r="F85" s="57"/>
       <c r="G85" s="16"/>
-      <c r="H85" s="53"/>
-      <c r="I85" s="53"/>
-      <c r="J85" s="53"/>
-      <c r="K85" s="53"/>
-      <c r="L85" s="55"/>
-      <c r="M85" s="56"/>
+      <c r="H85" s="58"/>
+      <c r="I85" s="57"/>
+      <c r="J85" s="57"/>
+      <c r="K85" s="57"/>
+      <c r="L85" s="60"/>
+      <c r="M85" s="61"/>
     </row>
     <row r="86" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="54"/>
+      <c r="A86" s="59"/>
       <c r="B86" s="22"/>
       <c r="C86" s="16"/>
       <c r="D86" s="16"/>
-      <c r="E86" s="52"/>
-      <c r="F86" s="53"/>
+      <c r="E86" s="56"/>
+      <c r="F86" s="57"/>
       <c r="G86" s="16"/>
-      <c r="H86" s="53"/>
-      <c r="I86" s="53"/>
-      <c r="J86" s="53"/>
-      <c r="K86" s="53"/>
-      <c r="L86" s="55"/>
-      <c r="M86" s="56"/>
+      <c r="H86" s="58"/>
+      <c r="I86" s="57"/>
+      <c r="J86" s="57"/>
+      <c r="K86" s="57"/>
+      <c r="L86" s="60"/>
+      <c r="M86" s="61"/>
     </row>
     <row r="87" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="54"/>
+      <c r="A87" s="59"/>
       <c r="B87" s="22"/>
       <c r="C87" s="16"/>
       <c r="D87" s="16"/>
-      <c r="E87" s="65"/>
-      <c r="F87" s="66"/>
+      <c r="E87" s="72"/>
+      <c r="F87" s="73"/>
       <c r="G87" s="16"/>
-      <c r="H87" s="66"/>
-      <c r="I87" s="66"/>
-      <c r="J87" s="66"/>
-      <c r="K87" s="66"/>
-      <c r="L87" s="67"/>
-      <c r="M87" s="68"/>
+      <c r="H87" s="74"/>
+      <c r="I87" s="73"/>
+      <c r="J87" s="73"/>
+      <c r="K87" s="73"/>
+      <c r="L87" s="75"/>
+      <c r="M87" s="76"/>
     </row>
     <row r="88" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="54"/>
+      <c r="A88" s="59"/>
       <c r="B88" s="18"/>
       <c r="C88" s="16"/>
       <c r="D88" s="16"/>
-      <c r="E88" s="65"/>
-      <c r="F88" s="66"/>
+      <c r="E88" s="72"/>
+      <c r="F88" s="73"/>
       <c r="G88" s="16"/>
-      <c r="H88" s="66"/>
-      <c r="I88" s="66"/>
-      <c r="J88" s="66"/>
-      <c r="K88" s="66"/>
-      <c r="L88" s="67"/>
-      <c r="M88" s="68"/>
+      <c r="H88" s="74"/>
+      <c r="I88" s="73"/>
+      <c r="J88" s="73"/>
+      <c r="K88" s="73"/>
+      <c r="L88" s="75"/>
+      <c r="M88" s="76"/>
     </row>
     <row r="89" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="54"/>
+      <c r="A89" s="59"/>
       <c r="B89" s="34"/>
       <c r="C89" s="16"/>
       <c r="D89" s="16"/>
-      <c r="E89" s="52"/>
-      <c r="F89" s="53"/>
+      <c r="E89" s="56"/>
+      <c r="F89" s="57"/>
       <c r="G89" s="16"/>
-      <c r="H89" s="53"/>
-      <c r="I89" s="53"/>
-      <c r="J89" s="53"/>
-      <c r="K89" s="53"/>
-      <c r="L89" s="55"/>
-      <c r="M89" s="56"/>
+      <c r="H89" s="58"/>
+      <c r="I89" s="57"/>
+      <c r="J89" s="57"/>
+      <c r="K89" s="57"/>
+      <c r="L89" s="60"/>
+      <c r="M89" s="61"/>
     </row>
     <row r="90" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="54"/>
+      <c r="A90" s="59"/>
       <c r="B90" s="22"/>
       <c r="C90" s="16"/>
       <c r="D90" s="16"/>
-      <c r="E90" s="52"/>
-      <c r="F90" s="53"/>
+      <c r="E90" s="56"/>
+      <c r="F90" s="57"/>
       <c r="G90" s="16"/>
-      <c r="H90" s="53"/>
-      <c r="I90" s="53"/>
-      <c r="J90" s="53"/>
-      <c r="K90" s="53"/>
-      <c r="L90" s="55"/>
-      <c r="M90" s="56"/>
+      <c r="H90" s="58"/>
+      <c r="I90" s="57"/>
+      <c r="J90" s="57"/>
+      <c r="K90" s="57"/>
+      <c r="L90" s="60"/>
+      <c r="M90" s="61"/>
     </row>
     <row r="91" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="54"/>
+      <c r="A91" s="59"/>
       <c r="B91" s="22"/>
       <c r="C91" s="16"/>
       <c r="D91" s="16"/>
-      <c r="E91" s="65"/>
-      <c r="F91" s="66"/>
+      <c r="E91" s="72"/>
+      <c r="F91" s="73"/>
       <c r="G91" s="16"/>
-      <c r="H91" s="66"/>
-      <c r="I91" s="66"/>
-      <c r="J91" s="66"/>
-      <c r="K91" s="66"/>
-      <c r="L91" s="67"/>
-      <c r="M91" s="68"/>
+      <c r="H91" s="74"/>
+      <c r="I91" s="73"/>
+      <c r="J91" s="73"/>
+      <c r="K91" s="73"/>
+      <c r="L91" s="75"/>
+      <c r="M91" s="76"/>
     </row>
     <row r="92" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="54"/>
+      <c r="A92" s="59"/>
       <c r="B92" s="18"/>
       <c r="C92" s="16"/>
       <c r="D92" s="16"/>
-      <c r="E92" s="65"/>
-      <c r="F92" s="66"/>
+      <c r="E92" s="72"/>
+      <c r="F92" s="73"/>
       <c r="G92" s="16"/>
-      <c r="H92" s="66"/>
-      <c r="I92" s="66"/>
-      <c r="J92" s="66"/>
-      <c r="K92" s="66"/>
-      <c r="L92" s="67"/>
-      <c r="M92" s="68"/>
+      <c r="H92" s="74"/>
+      <c r="I92" s="73"/>
+      <c r="J92" s="73"/>
+      <c r="K92" s="73"/>
+      <c r="L92" s="75"/>
+      <c r="M92" s="76"/>
     </row>
     <row r="93" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="54"/>
+      <c r="A93" s="59"/>
       <c r="B93" s="34"/>
       <c r="C93" s="16"/>
       <c r="D93" s="16"/>
-      <c r="E93" s="52"/>
-      <c r="F93" s="53"/>
+      <c r="E93" s="56"/>
+      <c r="F93" s="57"/>
       <c r="G93" s="16"/>
-      <c r="H93" s="53"/>
-      <c r="I93" s="53"/>
-      <c r="J93" s="53"/>
-      <c r="K93" s="53"/>
-      <c r="L93" s="55"/>
-      <c r="M93" s="56"/>
+      <c r="H93" s="58"/>
+      <c r="I93" s="57"/>
+      <c r="J93" s="57"/>
+      <c r="K93" s="57"/>
+      <c r="L93" s="60"/>
+      <c r="M93" s="61"/>
     </row>
     <row r="94" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="54"/>
+      <c r="A94" s="59"/>
       <c r="B94" s="22"/>
       <c r="C94" s="16"/>
       <c r="D94" s="16"/>
-      <c r="E94" s="52"/>
-      <c r="F94" s="53"/>
+      <c r="E94" s="56"/>
+      <c r="F94" s="57"/>
       <c r="G94" s="16"/>
-      <c r="H94" s="53"/>
-      <c r="I94" s="53"/>
-      <c r="J94" s="53"/>
-      <c r="K94" s="53"/>
-      <c r="L94" s="55"/>
-      <c r="M94" s="56"/>
+      <c r="H94" s="58"/>
+      <c r="I94" s="57"/>
+      <c r="J94" s="57"/>
+      <c r="K94" s="57"/>
+      <c r="L94" s="60"/>
+      <c r="M94" s="61"/>
     </row>
     <row r="95" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="54"/>
+      <c r="A95" s="59"/>
       <c r="B95" s="22"/>
       <c r="C95" s="16"/>
       <c r="D95" s="16"/>
-      <c r="E95" s="65"/>
-      <c r="F95" s="66"/>
+      <c r="E95" s="72"/>
+      <c r="F95" s="73"/>
       <c r="G95" s="16"/>
-      <c r="H95" s="66"/>
-      <c r="I95" s="66"/>
-      <c r="J95" s="66"/>
-      <c r="K95" s="66"/>
-      <c r="L95" s="67"/>
-      <c r="M95" s="68"/>
+      <c r="H95" s="74"/>
+      <c r="I95" s="73"/>
+      <c r="J95" s="73"/>
+      <c r="K95" s="73"/>
+      <c r="L95" s="75"/>
+      <c r="M95" s="76"/>
     </row>
     <row r="96" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="54"/>
+      <c r="A96" s="59"/>
       <c r="B96" s="18"/>
       <c r="C96" s="16"/>
       <c r="D96" s="16"/>
-      <c r="E96" s="65"/>
-      <c r="F96" s="66"/>
+      <c r="E96" s="72"/>
+      <c r="F96" s="73"/>
       <c r="G96" s="16"/>
-      <c r="H96" s="66"/>
-      <c r="I96" s="66"/>
-      <c r="J96" s="66"/>
-      <c r="K96" s="66"/>
-      <c r="L96" s="67"/>
-      <c r="M96" s="68"/>
+      <c r="H96" s="74"/>
+      <c r="I96" s="73"/>
+      <c r="J96" s="73"/>
+      <c r="K96" s="73"/>
+      <c r="L96" s="75"/>
+      <c r="M96" s="76"/>
     </row>
     <row r="97" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="54"/>
+      <c r="A97" s="59"/>
       <c r="B97" s="34"/>
       <c r="C97" s="16"/>
       <c r="D97" s="16"/>
-      <c r="E97" s="52"/>
-      <c r="F97" s="53"/>
+      <c r="E97" s="56"/>
+      <c r="F97" s="57"/>
       <c r="G97" s="16"/>
-      <c r="H97" s="53"/>
-      <c r="I97" s="53"/>
-      <c r="J97" s="53"/>
-      <c r="K97" s="53"/>
-      <c r="L97" s="55"/>
-      <c r="M97" s="56"/>
+      <c r="H97" s="58"/>
+      <c r="I97" s="57"/>
+      <c r="J97" s="57"/>
+      <c r="K97" s="57"/>
+      <c r="L97" s="60"/>
+      <c r="M97" s="61"/>
     </row>
     <row r="98" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="54"/>
+      <c r="A98" s="59"/>
       <c r="B98" s="22"/>
       <c r="C98" s="16"/>
       <c r="D98" s="16"/>
-      <c r="E98" s="52"/>
-      <c r="F98" s="53"/>
+      <c r="E98" s="56"/>
+      <c r="F98" s="57"/>
       <c r="G98" s="16"/>
-      <c r="H98" s="53"/>
-      <c r="I98" s="53"/>
-      <c r="J98" s="53"/>
-      <c r="K98" s="53"/>
-      <c r="L98" s="55"/>
-      <c r="M98" s="56"/>
+      <c r="H98" s="58"/>
+      <c r="I98" s="57"/>
+      <c r="J98" s="57"/>
+      <c r="K98" s="57"/>
+      <c r="L98" s="60"/>
+      <c r="M98" s="61"/>
     </row>
     <row r="99" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="54"/>
+      <c r="A99" s="59"/>
       <c r="B99" s="22"/>
       <c r="C99" s="16"/>
       <c r="D99" s="16"/>
-      <c r="E99" s="65"/>
-      <c r="F99" s="66"/>
+      <c r="E99" s="72"/>
+      <c r="F99" s="73"/>
       <c r="G99" s="16"/>
-      <c r="H99" s="66"/>
-      <c r="I99" s="66"/>
-      <c r="J99" s="66"/>
-      <c r="K99" s="66"/>
-      <c r="L99" s="67"/>
-      <c r="M99" s="68"/>
+      <c r="H99" s="74"/>
+      <c r="I99" s="73"/>
+      <c r="J99" s="73"/>
+      <c r="K99" s="73"/>
+      <c r="L99" s="75"/>
+      <c r="M99" s="76"/>
     </row>
     <row r="100" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="54"/>
+      <c r="A100" s="59"/>
       <c r="B100" s="18"/>
       <c r="C100" s="16"/>
       <c r="D100" s="16"/>
-      <c r="E100" s="65"/>
-      <c r="F100" s="66"/>
+      <c r="E100" s="72"/>
+      <c r="F100" s="73"/>
       <c r="G100" s="16"/>
-      <c r="H100" s="66"/>
-      <c r="I100" s="66"/>
-      <c r="J100" s="66"/>
-      <c r="K100" s="66"/>
-      <c r="L100" s="67"/>
-      <c r="M100" s="68"/>
+      <c r="H100" s="74"/>
+      <c r="I100" s="73"/>
+      <c r="J100" s="73"/>
+      <c r="K100" s="73"/>
+      <c r="L100" s="75"/>
+      <c r="M100" s="76"/>
     </row>
     <row r="101" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="54"/>
+      <c r="A101" s="59"/>
       <c r="B101" s="34"/>
       <c r="C101" s="16"/>
       <c r="D101" s="16"/>
-      <c r="E101" s="52"/>
-      <c r="F101" s="53"/>
+      <c r="E101" s="56"/>
+      <c r="F101" s="57"/>
       <c r="G101" s="16"/>
-      <c r="H101" s="53"/>
-      <c r="I101" s="53"/>
-      <c r="J101" s="53"/>
-      <c r="K101" s="53"/>
-      <c r="L101" s="55"/>
-      <c r="M101" s="56"/>
+      <c r="H101" s="58"/>
+      <c r="I101" s="57"/>
+      <c r="J101" s="57"/>
+      <c r="K101" s="57"/>
+      <c r="L101" s="60"/>
+      <c r="M101" s="61"/>
     </row>
     <row r="102" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="54"/>
+      <c r="A102" s="59"/>
       <c r="B102" s="22"/>
       <c r="C102" s="16"/>
       <c r="D102" s="16"/>
-      <c r="E102" s="52"/>
-      <c r="F102" s="53"/>
+      <c r="E102" s="56"/>
+      <c r="F102" s="57"/>
       <c r="G102" s="16"/>
-      <c r="H102" s="53"/>
-      <c r="I102" s="53"/>
-      <c r="J102" s="53"/>
-      <c r="K102" s="53"/>
-      <c r="L102" s="55"/>
-      <c r="M102" s="56"/>
+      <c r="H102" s="58"/>
+      <c r="I102" s="57"/>
+      <c r="J102" s="57"/>
+      <c r="K102" s="57"/>
+      <c r="L102" s="60"/>
+      <c r="M102" s="61"/>
     </row>
     <row r="103" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="54"/>
+      <c r="A103" s="59"/>
       <c r="B103" s="22"/>
       <c r="C103" s="16"/>
       <c r="D103" s="16"/>
-      <c r="E103" s="65"/>
-      <c r="F103" s="66"/>
+      <c r="E103" s="72"/>
+      <c r="F103" s="73"/>
       <c r="G103" s="16"/>
-      <c r="H103" s="66"/>
-      <c r="I103" s="66"/>
-      <c r="J103" s="66"/>
-      <c r="K103" s="66"/>
-      <c r="L103" s="67"/>
-      <c r="M103" s="68"/>
+      <c r="H103" s="74"/>
+      <c r="I103" s="73"/>
+      <c r="J103" s="73"/>
+      <c r="K103" s="73"/>
+      <c r="L103" s="75"/>
+      <c r="M103" s="76"/>
     </row>
     <row r="104" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="54"/>
+      <c r="A104" s="59"/>
       <c r="B104" s="18"/>
       <c r="C104" s="16"/>
       <c r="D104" s="16"/>
-      <c r="E104" s="65"/>
-      <c r="F104" s="66"/>
+      <c r="E104" s="72"/>
+      <c r="F104" s="73"/>
       <c r="G104" s="16"/>
-      <c r="H104" s="66"/>
-      <c r="I104" s="66"/>
-      <c r="J104" s="66"/>
-      <c r="K104" s="66"/>
-      <c r="L104" s="67"/>
-      <c r="M104" s="68"/>
+      <c r="H104" s="74"/>
+      <c r="I104" s="73"/>
+      <c r="J104" s="73"/>
+      <c r="K104" s="73"/>
+      <c r="L104" s="75"/>
+      <c r="M104" s="76"/>
     </row>
     <row r="105" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="54"/>
+      <c r="A105" s="59"/>
       <c r="B105" s="34"/>
       <c r="C105" s="16"/>
       <c r="D105" s="16"/>
-      <c r="E105" s="52"/>
-      <c r="F105" s="53"/>
+      <c r="E105" s="56"/>
+      <c r="F105" s="57"/>
       <c r="G105" s="16"/>
-      <c r="H105" s="53"/>
-      <c r="I105" s="53"/>
-      <c r="J105" s="53"/>
-      <c r="K105" s="53"/>
-      <c r="L105" s="55"/>
-      <c r="M105" s="56"/>
+      <c r="H105" s="58"/>
+      <c r="I105" s="57"/>
+      <c r="J105" s="57"/>
+      <c r="K105" s="57"/>
+      <c r="L105" s="60"/>
+      <c r="M105" s="61"/>
     </row>
     <row r="106" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="54"/>
+      <c r="A106" s="59"/>
       <c r="B106" s="22"/>
       <c r="C106" s="16"/>
       <c r="D106" s="16"/>
-      <c r="E106" s="52"/>
-      <c r="F106" s="53"/>
+      <c r="E106" s="56"/>
+      <c r="F106" s="57"/>
       <c r="G106" s="16"/>
-      <c r="H106" s="53"/>
-      <c r="I106" s="53"/>
-      <c r="J106" s="53"/>
-      <c r="K106" s="53"/>
-      <c r="L106" s="55"/>
-      <c r="M106" s="56"/>
+      <c r="H106" s="58"/>
+      <c r="I106" s="57"/>
+      <c r="J106" s="57"/>
+      <c r="K106" s="57"/>
+      <c r="L106" s="60"/>
+      <c r="M106" s="61"/>
     </row>
     <row r="107" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="54"/>
+      <c r="A107" s="59"/>
       <c r="B107" s="22"/>
       <c r="C107" s="16"/>
       <c r="D107" s="16"/>
-      <c r="E107" s="65"/>
-      <c r="F107" s="66"/>
+      <c r="E107" s="72"/>
+      <c r="F107" s="73"/>
       <c r="G107" s="16"/>
-      <c r="H107" s="66"/>
-      <c r="I107" s="66"/>
-      <c r="J107" s="66"/>
-      <c r="K107" s="66"/>
-      <c r="L107" s="67"/>
-      <c r="M107" s="68"/>
+      <c r="H107" s="74"/>
+      <c r="I107" s="73"/>
+      <c r="J107" s="73"/>
+      <c r="K107" s="73"/>
+      <c r="L107" s="75"/>
+      <c r="M107" s="76"/>
     </row>
     <row r="108" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="54"/>
+      <c r="A108" s="59"/>
       <c r="B108" s="18"/>
       <c r="C108" s="16"/>
       <c r="D108" s="16"/>
-      <c r="E108" s="65"/>
-      <c r="F108" s="66"/>
+      <c r="E108" s="72"/>
+      <c r="F108" s="73"/>
       <c r="G108" s="16"/>
-      <c r="H108" s="66"/>
-      <c r="I108" s="66"/>
-      <c r="J108" s="66"/>
-      <c r="K108" s="66"/>
-      <c r="L108" s="67"/>
-      <c r="M108" s="68"/>
+      <c r="H108" s="74"/>
+      <c r="I108" s="73"/>
+      <c r="J108" s="73"/>
+      <c r="K108" s="73"/>
+      <c r="L108" s="75"/>
+      <c r="M108" s="76"/>
     </row>
     <row r="109" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="54"/>
+      <c r="A109" s="59"/>
       <c r="B109" s="34"/>
       <c r="C109" s="16"/>
       <c r="D109" s="16"/>
-      <c r="E109" s="52"/>
-      <c r="F109" s="53"/>
+      <c r="E109" s="56"/>
+      <c r="F109" s="57"/>
       <c r="G109" s="16"/>
-      <c r="H109" s="53"/>
-      <c r="I109" s="53"/>
-      <c r="J109" s="53"/>
-      <c r="K109" s="53"/>
-      <c r="L109" s="55"/>
-      <c r="M109" s="56"/>
+      <c r="H109" s="58"/>
+      <c r="I109" s="57"/>
+      <c r="J109" s="57"/>
+      <c r="K109" s="57"/>
+      <c r="L109" s="60"/>
+      <c r="M109" s="61"/>
     </row>
     <row r="110" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="54"/>
+      <c r="A110" s="59"/>
       <c r="B110" s="22"/>
       <c r="C110" s="16"/>
       <c r="D110" s="16"/>
-      <c r="E110" s="52"/>
-      <c r="F110" s="53"/>
+      <c r="E110" s="56"/>
+      <c r="F110" s="57"/>
       <c r="G110" s="16"/>
-      <c r="H110" s="53"/>
-      <c r="I110" s="53"/>
-      <c r="J110" s="53"/>
-      <c r="K110" s="53"/>
-      <c r="L110" s="55"/>
-      <c r="M110" s="56"/>
+      <c r="H110" s="58"/>
+      <c r="I110" s="57"/>
+      <c r="J110" s="57"/>
+      <c r="K110" s="57"/>
+      <c r="L110" s="60"/>
+      <c r="M110" s="61"/>
     </row>
     <row r="111" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="54"/>
+      <c r="A111" s="59"/>
       <c r="B111" s="22"/>
       <c r="C111" s="16"/>
       <c r="D111" s="16"/>
-      <c r="E111" s="65"/>
-      <c r="F111" s="66"/>
+      <c r="E111" s="72"/>
+      <c r="F111" s="73"/>
       <c r="G111" s="16"/>
-      <c r="H111" s="66"/>
-      <c r="I111" s="66"/>
-      <c r="J111" s="66"/>
-      <c r="K111" s="66"/>
-      <c r="L111" s="67"/>
-      <c r="M111" s="68"/>
+      <c r="H111" s="74"/>
+      <c r="I111" s="73"/>
+      <c r="J111" s="73"/>
+      <c r="K111" s="73"/>
+      <c r="L111" s="75"/>
+      <c r="M111" s="76"/>
     </row>
     <row r="112" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="54"/>
+      <c r="A112" s="59"/>
       <c r="B112" s="18"/>
       <c r="C112" s="16"/>
       <c r="D112" s="16"/>
-      <c r="E112" s="65"/>
-      <c r="F112" s="66"/>
+      <c r="E112" s="72"/>
+      <c r="F112" s="73"/>
       <c r="G112" s="16"/>
-      <c r="H112" s="66"/>
-      <c r="I112" s="66"/>
-      <c r="J112" s="66"/>
-      <c r="K112" s="66"/>
-      <c r="L112" s="67"/>
-      <c r="M112" s="68"/>
+      <c r="H112" s="74"/>
+      <c r="I112" s="73"/>
+      <c r="J112" s="73"/>
+      <c r="K112" s="73"/>
+      <c r="L112" s="75"/>
+      <c r="M112" s="76"/>
     </row>
     <row r="113" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="54"/>
+      <c r="A113" s="59"/>
       <c r="B113" s="34"/>
       <c r="C113" s="16"/>
       <c r="D113" s="16"/>
-      <c r="E113" s="52"/>
-      <c r="F113" s="53"/>
+      <c r="E113" s="56"/>
+      <c r="F113" s="57"/>
       <c r="G113" s="16"/>
-      <c r="H113" s="53"/>
-      <c r="I113" s="53"/>
-      <c r="J113" s="53"/>
-      <c r="K113" s="53"/>
-      <c r="L113" s="55"/>
-      <c r="M113" s="56"/>
+      <c r="H113" s="58"/>
+      <c r="I113" s="57"/>
+      <c r="J113" s="57"/>
+      <c r="K113" s="57"/>
+      <c r="L113" s="60"/>
+      <c r="M113" s="61"/>
     </row>
     <row r="114" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="54"/>
+      <c r="A114" s="59"/>
       <c r="B114" s="22"/>
       <c r="C114" s="16"/>
       <c r="D114" s="16"/>
-      <c r="E114" s="52"/>
-      <c r="F114" s="53"/>
+      <c r="E114" s="56"/>
+      <c r="F114" s="57"/>
       <c r="G114" s="16"/>
-      <c r="H114" s="53"/>
-      <c r="I114" s="53"/>
-      <c r="J114" s="53"/>
-      <c r="K114" s="53"/>
-      <c r="L114" s="55"/>
-      <c r="M114" s="56"/>
+      <c r="H114" s="58"/>
+      <c r="I114" s="57"/>
+      <c r="J114" s="57"/>
+      <c r="K114" s="57"/>
+      <c r="L114" s="60"/>
+      <c r="M114" s="61"/>
     </row>
     <row r="115" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="54"/>
+      <c r="A115" s="59"/>
       <c r="B115" s="22"/>
       <c r="C115" s="16"/>
       <c r="D115" s="16"/>
-      <c r="E115" s="65"/>
-      <c r="F115" s="66"/>
+      <c r="E115" s="72"/>
+      <c r="F115" s="73"/>
       <c r="G115" s="16"/>
-      <c r="H115" s="66"/>
-      <c r="I115" s="66"/>
-      <c r="J115" s="66"/>
-      <c r="K115" s="66"/>
-      <c r="L115" s="67"/>
-      <c r="M115" s="68"/>
+      <c r="H115" s="74"/>
+      <c r="I115" s="73"/>
+      <c r="J115" s="73"/>
+      <c r="K115" s="73"/>
+      <c r="L115" s="75"/>
+      <c r="M115" s="76"/>
     </row>
     <row r="116" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="54"/>
+      <c r="A116" s="59"/>
       <c r="B116" s="18"/>
       <c r="C116" s="16"/>
       <c r="D116" s="16"/>
-      <c r="E116" s="65"/>
-      <c r="F116" s="66"/>
+      <c r="E116" s="72"/>
+      <c r="F116" s="73"/>
       <c r="G116" s="16"/>
-      <c r="H116" s="66"/>
-      <c r="I116" s="66"/>
-      <c r="J116" s="66"/>
-      <c r="K116" s="66"/>
-      <c r="L116" s="67"/>
-      <c r="M116" s="68"/>
+      <c r="H116" s="74"/>
+      <c r="I116" s="73"/>
+      <c r="J116" s="73"/>
+      <c r="K116" s="73"/>
+      <c r="L116" s="75"/>
+      <c r="M116" s="76"/>
     </row>
     <row r="117" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="54"/>
+      <c r="A117" s="59"/>
       <c r="B117" s="34"/>
       <c r="C117" s="16"/>
       <c r="D117" s="16"/>
-      <c r="E117" s="52"/>
-      <c r="F117" s="53"/>
+      <c r="E117" s="56"/>
+      <c r="F117" s="57"/>
       <c r="G117" s="16"/>
-      <c r="H117" s="53"/>
-      <c r="I117" s="53"/>
-      <c r="J117" s="53"/>
-      <c r="K117" s="53"/>
-      <c r="L117" s="55"/>
-      <c r="M117" s="56"/>
+      <c r="H117" s="58"/>
+      <c r="I117" s="57"/>
+      <c r="J117" s="57"/>
+      <c r="K117" s="57"/>
+      <c r="L117" s="60"/>
+      <c r="M117" s="61"/>
     </row>
     <row r="118" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="54"/>
+      <c r="A118" s="59"/>
       <c r="B118" s="22"/>
       <c r="C118" s="16"/>
       <c r="D118" s="16"/>
-      <c r="E118" s="52"/>
-      <c r="F118" s="53"/>
+      <c r="E118" s="56"/>
+      <c r="F118" s="57"/>
       <c r="G118" s="16"/>
-      <c r="H118" s="53"/>
-      <c r="I118" s="53"/>
-      <c r="J118" s="53"/>
-      <c r="K118" s="53"/>
-      <c r="L118" s="55"/>
-      <c r="M118" s="56"/>
+      <c r="H118" s="58"/>
+      <c r="I118" s="57"/>
+      <c r="J118" s="57"/>
+      <c r="K118" s="57"/>
+      <c r="L118" s="60"/>
+      <c r="M118" s="61"/>
     </row>
     <row r="119" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="54"/>
+      <c r="A119" s="59"/>
       <c r="B119" s="22"/>
       <c r="C119" s="16"/>
       <c r="D119" s="16"/>
-      <c r="E119" s="65"/>
-      <c r="F119" s="66"/>
+      <c r="E119" s="72"/>
+      <c r="F119" s="73"/>
       <c r="G119" s="16"/>
-      <c r="H119" s="66"/>
-      <c r="I119" s="66"/>
-      <c r="J119" s="66"/>
-      <c r="K119" s="66"/>
-      <c r="L119" s="67"/>
-      <c r="M119" s="68"/>
+      <c r="H119" s="74"/>
+      <c r="I119" s="73"/>
+      <c r="J119" s="73"/>
+      <c r="K119" s="73"/>
+      <c r="L119" s="75"/>
+      <c r="M119" s="76"/>
     </row>
     <row r="120" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="54"/>
+      <c r="A120" s="59"/>
       <c r="B120" s="18"/>
       <c r="C120" s="16"/>
       <c r="D120" s="16"/>
-      <c r="E120" s="65"/>
-      <c r="F120" s="66"/>
+      <c r="E120" s="72"/>
+      <c r="F120" s="73"/>
       <c r="G120" s="16"/>
-      <c r="H120" s="66"/>
-      <c r="I120" s="66"/>
-      <c r="J120" s="66"/>
-      <c r="K120" s="66"/>
-      <c r="L120" s="67"/>
-      <c r="M120" s="68"/>
+      <c r="H120" s="74"/>
+      <c r="I120" s="73"/>
+      <c r="J120" s="73"/>
+      <c r="K120" s="73"/>
+      <c r="L120" s="75"/>
+      <c r="M120" s="76"/>
     </row>
     <row r="121" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="54"/>
+      <c r="A121" s="59"/>
       <c r="B121" s="34"/>
       <c r="C121" s="16"/>
       <c r="D121" s="16"/>
-      <c r="E121" s="52"/>
-      <c r="F121" s="53"/>
+      <c r="E121" s="56"/>
+      <c r="F121" s="57"/>
       <c r="G121" s="16"/>
-      <c r="H121" s="53"/>
-      <c r="I121" s="53"/>
-      <c r="J121" s="53"/>
-      <c r="K121" s="53"/>
-      <c r="L121" s="55"/>
-      <c r="M121" s="56"/>
+      <c r="H121" s="58"/>
+      <c r="I121" s="57"/>
+      <c r="J121" s="57"/>
+      <c r="K121" s="57"/>
+      <c r="L121" s="60"/>
+      <c r="M121" s="61"/>
     </row>
     <row r="122" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="54"/>
+      <c r="A122" s="59"/>
       <c r="B122" s="22"/>
       <c r="C122" s="16"/>
       <c r="D122" s="16"/>
-      <c r="E122" s="52"/>
-      <c r="F122" s="53"/>
+      <c r="E122" s="56"/>
+      <c r="F122" s="57"/>
       <c r="G122" s="16"/>
-      <c r="H122" s="53"/>
-      <c r="I122" s="53"/>
-      <c r="J122" s="53"/>
-      <c r="K122" s="53"/>
-      <c r="L122" s="55"/>
-      <c r="M122" s="56"/>
+      <c r="H122" s="58"/>
+      <c r="I122" s="57"/>
+      <c r="J122" s="57"/>
+      <c r="K122" s="57"/>
+      <c r="L122" s="60"/>
+      <c r="M122" s="61"/>
     </row>
     <row r="123" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="54"/>
+      <c r="A123" s="59"/>
       <c r="B123" s="22"/>
       <c r="C123" s="16"/>
       <c r="D123" s="16"/>
-      <c r="E123" s="65"/>
-      <c r="F123" s="66"/>
+      <c r="E123" s="72"/>
+      <c r="F123" s="73"/>
       <c r="G123" s="16"/>
-      <c r="H123" s="66"/>
-      <c r="I123" s="66"/>
-      <c r="J123" s="66"/>
-      <c r="K123" s="66"/>
-      <c r="L123" s="67"/>
-      <c r="M123" s="68"/>
+      <c r="H123" s="74"/>
+      <c r="I123" s="73"/>
+      <c r="J123" s="73"/>
+      <c r="K123" s="73"/>
+      <c r="L123" s="75"/>
+      <c r="M123" s="76"/>
     </row>
     <row r="124" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="54"/>
+      <c r="A124" s="59"/>
       <c r="B124" s="18"/>
       <c r="C124" s="16"/>
       <c r="D124" s="16"/>
-      <c r="E124" s="65"/>
-      <c r="F124" s="66"/>
+      <c r="E124" s="72"/>
+      <c r="F124" s="73"/>
       <c r="G124" s="16"/>
-      <c r="H124" s="66"/>
-      <c r="I124" s="66"/>
-      <c r="J124" s="66"/>
-      <c r="K124" s="66"/>
-      <c r="L124" s="67"/>
-      <c r="M124" s="68"/>
+      <c r="H124" s="74"/>
+      <c r="I124" s="73"/>
+      <c r="J124" s="73"/>
+      <c r="K124" s="73"/>
+      <c r="L124" s="75"/>
+      <c r="M124" s="76"/>
     </row>
     <row r="125" spans="1:13" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="50"/>
+      <c r="A125" s="54"/>
       <c r="B125" s="22"/>
       <c r="C125" s="16"/>
       <c r="D125" s="16"/>
-      <c r="E125" s="52"/>
-      <c r="F125" s="53"/>
+      <c r="E125" s="56"/>
+      <c r="F125" s="57"/>
       <c r="G125" s="16"/>
-      <c r="H125" s="53"/>
-      <c r="I125" s="53"/>
-      <c r="J125" s="53"/>
-      <c r="K125" s="53"/>
-      <c r="L125" s="55"/>
-      <c r="M125" s="56"/>
+      <c r="H125" s="58"/>
+      <c r="I125" s="57"/>
+      <c r="J125" s="57"/>
+      <c r="K125" s="57"/>
+      <c r="L125" s="60"/>
+      <c r="M125" s="61"/>
     </row>
     <row r="126" spans="1:13" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="50"/>
+      <c r="A126" s="54"/>
       <c r="B126" s="22"/>
       <c r="C126" s="16"/>
       <c r="D126" s="16"/>
-      <c r="E126" s="52"/>
-      <c r="F126" s="53"/>
+      <c r="E126" s="56"/>
+      <c r="F126" s="57"/>
       <c r="G126" s="16"/>
-      <c r="H126" s="53"/>
-      <c r="I126" s="53"/>
-      <c r="J126" s="53"/>
-      <c r="K126" s="53"/>
-      <c r="L126" s="55"/>
-      <c r="M126" s="56"/>
+      <c r="H126" s="58"/>
+      <c r="I126" s="57"/>
+      <c r="J126" s="57"/>
+      <c r="K126" s="57"/>
+      <c r="L126" s="60"/>
+      <c r="M126" s="61"/>
     </row>
     <row r="127" spans="1:13" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="50"/>
+      <c r="A127" s="54"/>
       <c r="B127" s="22"/>
       <c r="C127" s="16"/>
       <c r="D127" s="16"/>
-      <c r="E127" s="57"/>
-      <c r="F127" s="59"/>
+      <c r="E127" s="62"/>
+      <c r="F127" s="64"/>
       <c r="G127" s="19"/>
-      <c r="H127" s="59"/>
-      <c r="I127" s="59"/>
-      <c r="J127" s="59"/>
-      <c r="K127" s="59"/>
-      <c r="L127" s="61"/>
-      <c r="M127" s="63"/>
+      <c r="H127" s="66"/>
+      <c r="I127" s="64"/>
+      <c r="J127" s="64"/>
+      <c r="K127" s="64"/>
+      <c r="L127" s="68"/>
+      <c r="M127" s="70"/>
     </row>
     <row r="128" spans="1:13" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="51"/>
+      <c r="A128" s="55"/>
       <c r="B128" s="22"/>
       <c r="C128" s="20"/>
       <c r="D128" s="21"/>
-      <c r="E128" s="58"/>
-      <c r="F128" s="60"/>
+      <c r="E128" s="63"/>
+      <c r="F128" s="65"/>
       <c r="G128" s="20"/>
-      <c r="H128" s="60"/>
-      <c r="I128" s="60"/>
-      <c r="J128" s="60"/>
-      <c r="K128" s="60"/>
-      <c r="L128" s="62"/>
-      <c r="M128" s="64"/>
+      <c r="H128" s="67"/>
+      <c r="I128" s="65"/>
+      <c r="J128" s="65"/>
+      <c r="K128" s="65"/>
+      <c r="L128" s="69"/>
+      <c r="M128" s="71"/>
     </row>
     <row r="129" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="77"/>
+      <c r="A129" s="86"/>
       <c r="B129" s="23" t="s">
         <v>17</v>
       </c>
@@ -3491,12 +3515,12 @@
         <v>20</v>
       </c>
       <c r="D129" s="23"/>
-      <c r="E129" s="80"/>
-      <c r="F129" s="48" t="s">
+      <c r="E129" s="89"/>
+      <c r="F129" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="G129" s="49"/>
-      <c r="H129" s="24"/>
+      <c r="G129" s="53"/>
+      <c r="H129" s="92"/>
       <c r="I129" s="24"/>
       <c r="J129" s="24"/>
       <c r="K129" s="24"/>
@@ -3504,7 +3528,7 @@
       <c r="M129" s="25"/>
     </row>
     <row r="130" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="78"/>
+      <c r="A130" s="87"/>
       <c r="B130" s="26" t="s">
         <v>18</v>
       </c>
@@ -3512,7 +3536,7 @@
         <v>21</v>
       </c>
       <c r="D130" s="26"/>
-      <c r="E130" s="81"/>
+      <c r="E130" s="90"/>
       <c r="F130" s="36" t="s">
         <v>15</v>
       </c>
@@ -3525,7 +3549,7 @@
       <c r="M130" s="29"/>
     </row>
     <row r="131" spans="1:13" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="79"/>
+      <c r="A131" s="88"/>
       <c r="B131" s="30" t="s">
         <v>19</v>
       </c>
@@ -3533,7 +3557,7 @@
         <v>22</v>
       </c>
       <c r="D131" s="30"/>
-      <c r="E131" s="82"/>
+      <c r="E131" s="91"/>
       <c r="F131" s="39" t="s">
         <v>16</v>
       </c>

</xml_diff>